<commit_message>
SimpleSheets 0.2.0 added support for more field types, hyper links and more cell styling
</commit_message>
<xml_diff>
--- a/test/FullExample.xlsx
+++ b/test/FullExample.xlsx
@@ -9,6 +9,7 @@
     <x:sheet name="Simple Fields" sheetId="2" r:id="rId2"/>
     <x:sheet name="Added Headers" sheetId="3" r:id="rId3"/>
     <x:sheet name="Styled Rows" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Adding Links" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <x:si>
     <x:t>Zaid</x:t>
   </x:si>
@@ -34,6 +35,12 @@
   </x:si>
   <x:si>
     <x:t>Active</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Github</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.github.com/</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -43,7 +50,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="3">
+  <x:fonts count="4">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -63,6 +70,14 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:u val="single"/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color theme="10"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
@@ -109,7 +124,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="5">
+  <x:cellStyleXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -125,8 +140,11 @@
     <x:xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -144,6 +162,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -616,4 +638,36 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B1" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="A1" r:id="rId8"/>
+    <x:hyperlink ref="B1" r:id="rId9"/>
+  </x:hyperlinks>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
SimpleSheets v0.3.0 better support for optional types
</commit_message>
<xml_diff>
--- a/test/FullExample.xlsx
+++ b/test/FullExample.xlsx
@@ -17,14 +17,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <x:si>
     <x:t>Zaid</x:t>
   </x:si>
   <x:si>
+    <x:t>Ajaj</x:t>
+  </x:si>
+  <x:si>
     <x:t>Jane</x:t>
   </x:si>
   <x:si>
+    <x:t>Doe</x:t>
+  </x:si>
+  <x:si>
     <x:t>John</x:t>
   </x:si>
   <x:si>
@@ -34,7 +40,10 @@
     <x:t>Age</x:t>
   </x:si>
   <x:si>
-    <x:t>Active</x:t>
+    <x:t>Working</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DateOfBirth</x:t>
   </x:si>
   <x:si>
     <x:t>Github</x:t>
@@ -47,8 +56,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
+  <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
+    <x:numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </x:numFmts>
   <x:fonts count="4">
     <x:font>
@@ -124,16 +134,22 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="6">
+  <x:cellStyleXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -144,16 +160,24 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="6">
+  <x:cellXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -464,13 +488,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C3"/>
+  <x:dimension ref="A1:F3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -480,27 +504,45 @@
       <x:c r="C1" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3">
+      <x:c r="D1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E1" s="1">
+        <x:v>35382</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
         <x:v>26</x:v>
       </x:c>
       <x:c r="C2" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E2" s="1">
+        <x:v>43831</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>25</x:v>
       </x:c>
       <x:c r="C3" s="0" t="b">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="E3" s="1">
+        <x:v>43831</x:v>
+      </x:c>
+      <x:c r="F3" s="1">
+        <x:v>43831</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -525,13 +567,13 @@
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3">
@@ -547,18 +589,18 @@
     </x:row>
     <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>26</x:v>
       </x:c>
       <x:c r="C3" s="0" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
         <x:v>25</x:v>
@@ -581,54 +623,66 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C4"/>
+  <x:dimension ref="A1:D4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3">
+      <x:c r="B1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="b">
+      <x:c r="C2" s="3" t="b">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
-      <x:c r="A3" s="3" t="s">
-        <x:v>1</x:v>
+      <x:c r="D2" s="4">
+        <x:v>35382</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C3" s="4" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="3" t="s">
-        <x:v>2</x:v>
+      <x:c r="C3" s="3" t="b">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D3" s="4">
+        <x:v>43831</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="5" t="s">
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C4" s="4" t="b">
+      <x:c r="C4" s="6" t="b">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="D4" s="4">
+        <x:v>43831</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -652,11 +706,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:2">
-      <x:c r="A1" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B1" s="5" t="s">
-        <x:v>7</x:v>
+      <x:c r="A1" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B1" s="7" t="s">
+        <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
SimpleSheets v0.4.0 added image support and more small improvements
</commit_message>
<xml_diff>
--- a/test/FullExample.xlsx
+++ b/test/FullExample.xlsx
@@ -10,6 +10,7 @@
     <x:sheet name="Added Headers" sheetId="3" r:id="rId3"/>
     <x:sheet name="Styled Rows" sheetId="4" r:id="rId4"/>
     <x:sheet name="Adding Links" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Images" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <x:si>
     <x:t>Zaid</x:t>
   </x:si>
@@ -50,6 +51,18 @@
   </x:si>
   <x:si>
     <x:t>https://www.github.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Year overview</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Line chart</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bar chart</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -160,7 +173,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="8">
+  <x:cellXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -191,6 +204,14 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -198,6 +219,83 @@
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
 </x:styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4762500" cy="4762500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect"/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4762500" cy="4762500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect"/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,8 +591,13 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="11.950625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="9.830625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:6" customFormat="1" ht="15.218096" customHeight="1">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -511,7 +614,7 @@
         <x:v>35382</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
+    <x:row r="2" spans="1:6" customFormat="1" ht="15.218096" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -528,7 +631,7 @@
         <x:v>43831</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:6">
+    <x:row r="3" spans="1:6" customFormat="1" ht="15.218096" customHeight="1">
       <x:c r="A3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -628,6 +731,10 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="3" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="12.060625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
@@ -643,7 +750,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
+    <x:row r="2" spans="1:4" customFormat="1" ht="15.218096" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -657,7 +764,7 @@
         <x:v>35382</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
+    <x:row r="3" spans="1:4" customFormat="1" ht="15.218096" customHeight="1">
       <x:c r="A3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -671,7 +778,7 @@
         <x:v>43831</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:4" customFormat="1" ht="15.218096" customHeight="1">
       <x:c r="A4" s="5" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -715,8 +822,8 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A1" r:id="rId8"/>
-    <x:hyperlink ref="B1" r:id="rId9"/>
+    <x:hyperlink ref="A1" r:id="rId9"/>
+    <x:hyperlink ref="B1" r:id="rId10"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -724,4 +831,47 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C4"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="15.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="40.710625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="8" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B1" s="8" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3" customFormat="1" ht="60" customHeight="1">
+      <x:c r="A2" s="9" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3" customFormat="1" ht="60" customHeight="1">
+      <x:c r="A3" s="9" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
SimpleSheets v0.6.0 Improved type-inference through the use of extension methods
</commit_message>
<xml_diff>
--- a/test/FullExample.xlsx
+++ b/test/FullExample.xlsx
@@ -7,10 +7,11 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Simple Fields" sheetId="2" r:id="rId2"/>
-    <x:sheet name="Added Headers" sheetId="3" r:id="rId3"/>
-    <x:sheet name="Styled Rows" sheetId="4" r:id="rId4"/>
-    <x:sheet name="Adding Links" sheetId="5" r:id="rId5"/>
-    <x:sheet name="Images" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Inferred Fields" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Added Headers" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Styled Rows" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Adding Links" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Images" sheetId="7" r:id="rId7"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -244,7 +245,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12" cstate="print"/>
+        <a:blip r:embed="rId13" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -280,7 +281,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13" cstate="print"/>
+        <a:blip r:embed="rId14" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -662,6 +663,82 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
+  <x:dimension ref="A1:F3"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="11.950625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="9.830625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:6" customFormat="1" ht="15.218096" customHeight="1">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E1" s="1">
+        <x:v>35382</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" customFormat="1" ht="15.218096" customHeight="1">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E2" s="1">
+        <x:v>43831</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" customFormat="1" ht="15.218096" customHeight="1">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E3" s="1">
+        <x:v>43831</x:v>
+      </x:c>
+      <x:c r="F3" s="1">
+        <x:v>43831</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
   <x:dimension ref="A1:C4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -721,7 +798,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -801,7 +878,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -822,8 +899,8 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A1" r:id="rId9"/>
-    <x:hyperlink ref="B1" r:id="rId10"/>
+    <x:hyperlink ref="A1" r:id="rId10"/>
+    <x:hyperlink ref="B1" r:id="rId11"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -833,7 +910,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -871,7 +948,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Better charts generated from the test project
</commit_message>
<xml_diff>
--- a/test/FullExample.xlsx
+++ b/test/FullExample.xlsx
@@ -922,7 +922,7 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="15.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="40.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="50.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3">
@@ -933,12 +933,12 @@
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:3" customFormat="1" ht="60" customHeight="1">
+    <x:row r="2" spans="1:3" customFormat="1" ht="80" customHeight="1">
       <x:c r="A2" s="9" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:3" customFormat="1" ht="60" customHeight="1">
+    <x:row r="3" spans="1:3" customFormat="1" ht="80" customHeight="1">
       <x:c r="A3" s="9" t="s">
         <x:v>14</x:v>
       </x:c>

</xml_diff>